<commit_message>
Updated SSL Lab report and Progress TRacker
</commit_message>
<xml_diff>
--- a/Documents/Progress Tracker.xlsx
+++ b/Documents/Progress Tracker.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>#</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Phase 1: Approx End Date - 3rd March. Exp O/P - Necessary R&amp;D completed. Design &amp; Documentation completed. Server Setup Completed.</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -75,7 +78,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -85,6 +88,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -116,7 +125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -137,6 +146,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,7 +433,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,10 +450,10 @@
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="4"/>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="5"/>
+      <c r="D1" s="6"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -452,10 +465,10 @@
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -475,13 +488,15 @@
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="8">
         <v>1.5</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="8">
         <v>1.5</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
@@ -492,10 +507,10 @@
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>2</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>2</v>
       </c>
       <c r="E4" s="3"/>
@@ -509,10 +524,10 @@
       <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>24</v>
       </c>
-      <c r="D5" s="6"/>
+      <c r="D5" s="5"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -524,8 +539,8 @@
       <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6">
+      <c r="C6" s="5"/>
+      <c r="D6" s="5">
         <v>24</v>
       </c>
       <c r="E6" s="3"/>

</xml_diff>

<commit_message>
Created initial database design document
</commit_message>
<xml_diff>
--- a/Documents/Progress Tracker.xlsx
+++ b/Documents/Progress Tracker.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17870"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>#</t>
   </si>
@@ -45,24 +45,19 @@
     <t>Plan Date</t>
   </si>
   <si>
-    <t>Flow Chart of a whole System - Brainstorming</t>
-  </si>
-  <si>
     <t>Estimation in hours</t>
   </si>
   <si>
-    <t>Documentation of Login, Registration, End-to-End Encryption. (UC, CD, SEQ etc)
-Design system by identifying Assets, stakeholders, adversary etc.</t>
-  </si>
-  <si>
-    <t>Documentation of Local chat storage protection, U2U authentication. (UC, CD, SEQ etc)
-Design system by identifying Assets, stakeholders, adversary etc.</t>
-  </si>
-  <si>
-    <t>Phase 1: Approx End Date - 3rd March. Exp O/P - Necessary R&amp;D completed. Design &amp; Documentation completed. Server Setup Completed.</t>
-  </si>
-  <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>Database Design Document</t>
+  </si>
+  <si>
+    <t>Registration Use-case and sequence diagram</t>
+  </si>
+  <si>
+    <t>Create tables in database and generate scripts</t>
   </si>
 </sst>
 </file>
@@ -78,18 +73,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -125,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -143,13 +132,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,10 +440,10 @@
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="4"/>
-      <c r="C1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="6"/>
+      <c r="C1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="9"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -488,14 +478,14 @@
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="10">
         <v>1.5</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="10">
         <v>1.5</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>13</v>
+      <c r="E3" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -505,63 +495,59 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="5">
+        <v>10</v>
+      </c>
+      <c r="C4" s="10">
         <v>2</v>
       </c>
-      <c r="D4" s="5">
-        <v>2</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="8">
+        <v>42802</v>
+      </c>
+      <c r="G4" s="8">
+        <v>42802</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="5">
-        <v>24</v>
-      </c>
-      <c r="D5" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="C5" s="10">
+        <v>1</v>
+      </c>
+      <c r="D5" s="10"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="F5" s="8">
+        <v>42802</v>
+      </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5">
-        <v>24</v>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6">
+        <v>8</v>
       </c>
       <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="F6" s="8">
+        <v>42803</v>
+      </c>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A7:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>